<commit_message>
Evaluate RAG system and modify README.md
</commit_message>
<xml_diff>
--- a/planner/521H0220_52100254.xlsx
+++ b/planner/521H0220_52100254.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\TDTU\ProjectIT\Chatbot_RAG_2024\planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40388C51-E829-4B35-8C66-BD9D2AD609B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80794F37-98D8-475F-B073-2CE66A49C1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D4BD54A8-8A29-490D-AE46-455AD473DFA0}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -168,65 +168,65 @@
     <t xml:space="preserve">Email: </t>
   </si>
   <si>
-    <t>Tìm hiểu về cấu trúc RAG</t>
-  </si>
-  <si>
-    <t>Thu thập dữ liệu về luật giao thông đường bộ</t>
-  </si>
-  <si>
-    <t>Thu thập dữ liệu luật giao thông đường bộ</t>
-  </si>
-  <si>
-    <t>Thu thập dữ liệu luật giao thông đường bộ
-Tìm hiểu cấu trúc văn bản luật giao thông đường bộ</t>
-  </si>
-  <si>
-    <t>Thu thập thêm dữ liệu luật giao thông đường bộ
-Tìm hiểu cấu trúc luật và thử nghiệm chunking</t>
-  </si>
-  <si>
-    <t>Xây dụng thành công baseline cấu trúc RAG cơ bản sử dụng langchain</t>
-  </si>
-  <si>
-    <t>Thử nghiệm vectorstore</t>
-  </si>
-  <si>
-    <t>Xây dựng baseline hệ thống RAG cơ bản</t>
-  </si>
-  <si>
-    <t>Demo cơ bản hệ thống RAG trên streamlit</t>
-  </si>
-  <si>
-    <t>Hoàn thành demo cơ bản hệ thống RAG trên streamlit</t>
-  </si>
-  <si>
     <t>Cải thiện hệ thống RAG sử dụng kỹ thuật fewshot Chain of thought</t>
   </si>
   <si>
-    <t>Thực hiện prompting với kỹ thuật Fewshot chain of thought</t>
+    <t>- Thu thập dữ liệu về luật giao thông đường bộ</t>
   </si>
   <si>
-    <t>Cải thiện hệ thống RAG sử dụng kỹ thuật fewshot Chain of thought
-Thử nghiệm Parent Child retrieval trên postgres SQL</t>
+    <t>- Tìm hiểu về cấu trúc RAG</t>
   </si>
   <si>
-    <t>Thử nghiệm Vectorstore trên Pinecone và Postgres SQL</t>
+    <t>-Thử nghiệm vectorstore</t>
   </si>
   <si>
-    <t>Hoàn thành việc cải thiện RAG với fewshot Chain of thought
-Hoàn thành cấu hình Parent Child retrieval và lưu trữ data trên Postgres SQL</t>
+    <t>- Thu thập dữ liệu luật giao thông đường bộ
+- Tìm hiểu cấu trúc văn bản luật giao thông đường bộ</t>
   </si>
   <si>
-    <t xml:space="preserve">Điều chỉnh lại giao diện cho Streamlit </t>
+    <t>- Xây dựng baseline hệ thống RAG cơ bản</t>
   </si>
   <si>
-    <t>Hoàn thành việc điều chỉnh giao diện</t>
+    <t>- Demo cơ bản hệ thống RAG trên streamlit</t>
   </si>
   <si>
-    <t>Hoàn thiện phần code và report</t>
+    <t>- Cải thiện hệ thống RAG sử dụng kỹ thuật fewshot Chain of thought
+- Thử nghiệm Parent Child retrieval trên postgres SQL</t>
   </si>
   <si>
-    <t>Hoàn thành việc hoàn thiện code và report</t>
+    <t xml:space="preserve">- Điều chỉnh lại giao diện cho Streamlit </t>
+  </si>
+  <si>
+    <t>- Thu thập dữ liệu luật giao thông đường bộ</t>
+  </si>
+  <si>
+    <t>- Thu thập thêm dữ liệu luật giao thông đường bộ
+- Tìm hiểu cấu trúc luật và thử nghiệm chunking</t>
+  </si>
+  <si>
+    <t>- Thử nghiệm Vectorstore trên Pinecone và Postgres SQL</t>
+  </si>
+  <si>
+    <t>- Xây dụng thành công baseline cấu trúc RAG cơ bản sử dụng langchain</t>
+  </si>
+  <si>
+    <t>- Hoàn thành demo cơ bản hệ thống RAG trên streamlit</t>
+  </si>
+  <si>
+    <t>- Thực hiện prompting với kỹ thuật Fewshot chain of thought</t>
+  </si>
+  <si>
+    <t>- Hoàn thành việc cải thiện RAG với fewshot Chain of thought
+- Hoàn thành cấu hình Parent Child retrieval và lưu trữ data trên Postgres SQL</t>
+  </si>
+  <si>
+    <t>- Hoàn thành việc điều chỉnh giao diện</t>
+  </si>
+  <si>
+    <t>- Hoàn thiện phần code và report</t>
+  </si>
+  <si>
+    <t>- Hoàn thành việc hoàn thiện code và report</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -478,6 +478,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -519,8 +522,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -544,15 +550,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>1234440</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>51435</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3596640</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>36195</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -582,7 +588,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5311140" y="10020300"/>
+          <a:off x="9570720" y="10927080"/>
           <a:ext cx="2362200" cy="904875"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -899,27 +905,28 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y1007"/>
+  <dimension ref="A1:Y1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31:F31"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="5" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="79" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="7" customFormat="1" ht="41.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -943,14 +950,14 @@
       <c r="Y1" s="6"/>
     </row>
     <row r="2" spans="1:25" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -1000,11 +1007,11 @@
     </row>
     <row r="4" spans="1:25" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1060,10 +1067,10 @@
     </row>
     <row r="6" spans="1:25" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="23"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="13" t="s">
         <v>25</v>
       </c>
@@ -1124,10 +1131,10 @@
     </row>
     <row r="8" spans="1:25" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="23"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="13" t="s">
         <v>27</v>
       </c>
@@ -1188,10 +1195,10 @@
     </row>
     <row r="10" spans="1:25" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1318,7 +1325,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="5">
-        <v>45604</v>
+        <v>45598</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="2"/>
@@ -1420,11 +1427,11 @@
         <f>B17+6</f>
         <v>45604</v>
       </c>
-      <c r="D17" s="17" t="s">
-        <v>33</v>
+      <c r="D17" s="34" t="s">
+        <v>35</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>33</v>
+      <c r="E17" s="35" t="s">
+        <v>35</v>
       </c>
       <c r="F17" s="15">
         <v>1</v>
@@ -1449,7 +1456,7 @@
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
     </row>
-    <row r="18" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>2</v>
       </c>
@@ -1458,14 +1465,14 @@
         <v>45605</v>
       </c>
       <c r="C18" s="8">
-        <f t="shared" ref="C18:C32" si="0">B18+6</f>
+        <f t="shared" ref="C18:C33" si="0">B18+6</f>
         <v>45611</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="12" t="s">
-        <v>35</v>
+      <c r="E18" s="35" t="s">
+        <v>42</v>
       </c>
       <c r="F18" s="15">
         <v>0.2</v>
@@ -1490,7 +1497,7 @@
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
     </row>
-    <row r="19" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
         <v>3</v>
       </c>
@@ -1502,11 +1509,11 @@
         <f t="shared" si="0"/>
         <v>45618</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>36</v>
+      <c r="D19" s="34" t="s">
+        <v>37</v>
       </c>
-      <c r="E19" s="17" t="s">
-        <v>37</v>
+      <c r="E19" s="34" t="s">
+        <v>43</v>
       </c>
       <c r="F19" s="15">
         <v>1</v>
@@ -1543,11 +1550,11 @@
         <f t="shared" si="0"/>
         <v>45625</v>
       </c>
-      <c r="D20" s="12" t="s">
-        <v>39</v>
+      <c r="D20" s="35" t="s">
+        <v>36</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>46</v>
+      <c r="E20" s="35" t="s">
+        <v>44</v>
       </c>
       <c r="F20" s="15">
         <v>1</v>
@@ -1584,11 +1591,11 @@
         <f t="shared" si="0"/>
         <v>45632</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>40</v>
+      <c r="D21" s="35" t="s">
+        <v>38</v>
       </c>
-      <c r="E21" s="12" t="s">
-        <v>38</v>
+      <c r="E21" s="35" t="s">
+        <v>45</v>
       </c>
       <c r="F21" s="15">
         <v>1</v>
@@ -1625,11 +1632,11 @@
         <f t="shared" si="0"/>
         <v>45639</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>41</v>
+      <c r="D22" s="35" t="s">
+        <v>39</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>42</v>
+      <c r="E22" s="35" t="s">
+        <v>46</v>
       </c>
       <c r="F22" s="15">
         <v>1</v>
@@ -1659,7 +1666,7 @@
         <v>7</v>
       </c>
       <c r="B23" s="8">
-        <f t="shared" ref="B23:B32" si="2">B22+7</f>
+        <f t="shared" ref="B23:B33" si="2">B22+7</f>
         <v>45640</v>
       </c>
       <c r="C23" s="8">
@@ -1667,10 +1674,10 @@
         <v>45646</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
-      <c r="E23" s="12" t="s">
-        <v>44</v>
+      <c r="E23" s="35" t="s">
+        <v>47</v>
       </c>
       <c r="F23" s="15">
         <v>0.5</v>
@@ -1695,7 +1702,7 @@
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
     </row>
-    <row r="24" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A24" s="11">
         <v>8</v>
       </c>
@@ -1707,11 +1714,11 @@
         <f t="shared" si="0"/>
         <v>45653</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>45</v>
+      <c r="D24" s="34" t="s">
+        <v>40</v>
       </c>
-      <c r="E24" s="17" t="s">
-        <v>47</v>
+      <c r="E24" s="34" t="s">
+        <v>48</v>
       </c>
       <c r="F24" s="15">
         <v>1</v>
@@ -1748,10 +1755,10 @@
         <f t="shared" si="0"/>
         <v>45660</v>
       </c>
-      <c r="D25" s="17" t="s">
-        <v>48</v>
+      <c r="D25" s="34" t="s">
+        <v>41</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="34" t="s">
         <v>49</v>
       </c>
       <c r="F25" s="15">
@@ -1789,11 +1796,11 @@
         <f t="shared" si="0"/>
         <v>45667</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1826,11 +1833,11 @@
         <f t="shared" si="0"/>
         <v>45674</v>
       </c>
-      <c r="D27" s="24" t="s">
+      <c r="D27" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="25"/>
-      <c r="F27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="27"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -1863,9 +1870,9 @@
         <f t="shared" si="0"/>
         <v>45681</v>
       </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="29"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="30"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -1898,9 +1905,9 @@
         <f t="shared" si="0"/>
         <v>45688</v>
       </c>
-      <c r="D29" s="30"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="32"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="33"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -1923,20 +1930,20 @@
     </row>
     <row r="30" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
-        <v>9</v>
+        <v>14</v>
       </c>
-      <c r="B30" s="33">
-        <f t="shared" si="2"/>
+      <c r="B30" s="18">
+        <f>B29+7</f>
         <v>45689</v>
       </c>
       <c r="C30" s="8">
-        <f t="shared" ref="C30" si="3">B30+6</f>
+        <f t="shared" ref="C30:C31" si="3">B30+6</f>
         <v>45695</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="34" t="s">
         <v>51</v>
       </c>
       <c r="F30" s="15">
@@ -1963,22 +1970,18 @@
       <c r="Y30" s="2"/>
     </row>
     <row r="31" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="11">
-        <v>15</v>
-      </c>
-      <c r="B31" s="9">
+      <c r="A31" s="11"/>
+      <c r="B31" s="18">
         <f t="shared" si="2"/>
         <v>45696</v>
       </c>
-      <c r="C31" s="9">
-        <f t="shared" si="0"/>
+      <c r="C31" s="8">
+        <f t="shared" si="3"/>
         <v>45702</v>
       </c>
-      <c r="D31" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="15"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -2001,7 +2004,7 @@
     </row>
     <row r="32" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" s="9">
         <f t="shared" si="2"/>
@@ -2011,11 +2014,11 @@
         <f t="shared" si="0"/>
         <v>45709</v>
       </c>
-      <c r="D32" s="20" t="s">
-        <v>19</v>
+      <c r="D32" s="21" t="s">
+        <v>18</v>
       </c>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -2037,12 +2040,22 @@
       <c r="Y32" s="2"/>
     </row>
     <row r="33" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="A33" s="11">
+        <v>16</v>
+      </c>
+      <c r="B33" s="9">
+        <f t="shared" si="2"/>
+        <v>45710</v>
+      </c>
+      <c r="C33" s="9">
+        <f t="shared" si="0"/>
+        <v>45716</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -2064,13 +2077,11 @@
       <c r="Y33" s="2"/>
     </row>
     <row r="34" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -2092,12 +2103,14 @@
       <c r="X34" s="2"/>
       <c r="Y34" s="2"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+    <row r="35" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="19"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -2119,7 +2132,7 @@
       <c r="X35" s="2"/>
       <c r="Y35" s="2"/>
     </row>
-    <row r="36" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2146,7 +2159,7 @@
       <c r="X36" s="2"/>
       <c r="Y36" s="2"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -28310,6 +28323,12 @@
       <c r="Y1005" s="2"/>
     </row>
     <row r="1006" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1006" s="2"/>
+      <c r="B1006" s="2"/>
+      <c r="C1006" s="2"/>
+      <c r="D1006" s="2"/>
+      <c r="E1006" s="2"/>
+      <c r="F1006" s="2"/>
       <c r="G1006" s="2"/>
       <c r="H1006" s="2"/>
       <c r="I1006" s="2"/>
@@ -28351,9 +28370,30 @@
       <c r="X1007" s="2"/>
       <c r="Y1007" s="2"/>
     </row>
+    <row r="1008" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="G1008" s="2"/>
+      <c r="H1008" s="2"/>
+      <c r="I1008" s="2"/>
+      <c r="J1008" s="2"/>
+      <c r="K1008" s="2"/>
+      <c r="L1008" s="2"/>
+      <c r="M1008" s="2"/>
+      <c r="N1008" s="2"/>
+      <c r="O1008" s="2"/>
+      <c r="P1008" s="2"/>
+      <c r="Q1008" s="2"/>
+      <c r="R1008" s="2"/>
+      <c r="S1008" s="2"/>
+      <c r="T1008" s="2"/>
+      <c r="U1008" s="2"/>
+      <c r="V1008" s="2"/>
+      <c r="W1008" s="2"/>
+      <c r="X1008" s="2"/>
+      <c r="Y1008" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:C35"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A2:F2"/>
@@ -28361,8 +28401,8 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D31:F31"/>
     <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
     <mergeCell ref="D27:F29"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.37" bottom="0.2" header="0.3" footer="0.3"/>

</xml_diff>